<commit_message>
add Shop, custom character hat
</commit_message>
<xml_diff>
--- a/Project2/map/map_stage0.xlsx
+++ b/Project2/map/map_stage0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files\Project2\Project2\map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JumpKing\Project2\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54576CB6-D460-4EFA-904D-DE675D216D89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C366973B-AFDA-4A69-A934-FCE8CDC82136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{43B2A935-9574-4456-95D9-363CC87949CB}"/>
   </bookViews>
@@ -22,10 +22,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,7 +65,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -87,16 +83,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -412,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF67B08-2CB8-4D9E-8CCD-07B2A0732180}">
   <dimension ref="A1:AN300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" zoomScale="69" workbookViewId="0">
-      <selection activeCell="BA284" sqref="BA284"/>
+    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="69" workbookViewId="0">
+      <selection activeCell="AR280" sqref="AR280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -423,129 +409,129 @@
   <sheetData>
     <row r="1" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="G1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="I1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="J1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="K1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="N1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="O1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="P1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="Q1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="R1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="S1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="T1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="U1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="V1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="W1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="Y1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="Z1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AA1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AB1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AC1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AD1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AE1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AF1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AG1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AH1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AI1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AJ1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AK1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AL1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AM1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="AN1" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -662,12 +648,12 @@
         <v>0</v>
       </c>
       <c r="AN2" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -784,12 +770,12 @@
         <v>0</v>
       </c>
       <c r="AN3" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -906,12 +892,12 @@
         <v>0</v>
       </c>
       <c r="AN4" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
@@ -1028,12 +1014,12 @@
         <v>0</v>
       </c>
       <c r="AN5" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1">
         <v>0</v>
@@ -1150,12 +1136,12 @@
         <v>0</v>
       </c>
       <c r="AN6" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -1272,12 +1258,12 @@
         <v>0</v>
       </c>
       <c r="AN7" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -1394,12 +1380,12 @@
         <v>0</v>
       </c>
       <c r="AN8" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -1516,12 +1502,12 @@
         <v>0</v>
       </c>
       <c r="AN9" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -1638,12 +1624,12 @@
         <v>0</v>
       </c>
       <c r="AN10" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -1760,12 +1746,12 @@
         <v>0</v>
       </c>
       <c r="AN11" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -1882,12 +1868,12 @@
         <v>0</v>
       </c>
       <c r="AN12" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -2004,12 +1990,12 @@
         <v>0</v>
       </c>
       <c r="AN13" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -2126,12 +2112,12 @@
         <v>0</v>
       </c>
       <c r="AN14" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -2248,12 +2234,12 @@
         <v>0</v>
       </c>
       <c r="AN15" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -2370,12 +2356,12 @@
         <v>0</v>
       </c>
       <c r="AN16" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -2492,12 +2478,12 @@
         <v>0</v>
       </c>
       <c r="AN17" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -2614,12 +2600,12 @@
         <v>0</v>
       </c>
       <c r="AN18" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -2736,12 +2722,12 @@
         <v>0</v>
       </c>
       <c r="AN19" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -2858,12 +2844,12 @@
         <v>0</v>
       </c>
       <c r="AN20" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -2980,12 +2966,12 @@
         <v>0</v>
       </c>
       <c r="AN21" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -3102,12 +3088,12 @@
         <v>0</v>
       </c>
       <c r="AN22" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -3224,12 +3210,12 @@
         <v>0</v>
       </c>
       <c r="AN23" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -3346,12 +3332,12 @@
         <v>0</v>
       </c>
       <c r="AN24" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -3468,12 +3454,12 @@
         <v>0</v>
       </c>
       <c r="AN25" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -3590,12 +3576,12 @@
         <v>0</v>
       </c>
       <c r="AN26" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -3712,12 +3698,12 @@
         <v>0</v>
       </c>
       <c r="AN27" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -3834,12 +3820,12 @@
         <v>0</v>
       </c>
       <c r="AN28" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -3956,12 +3942,12 @@
         <v>0</v>
       </c>
       <c r="AN29" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -4078,12 +4064,12 @@
         <v>0</v>
       </c>
       <c r="AN30" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -4200,12 +4186,12 @@
         <v>0</v>
       </c>
       <c r="AN31" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -4322,12 +4308,12 @@
         <v>0</v>
       </c>
       <c r="AN32" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -4444,12 +4430,12 @@
         <v>0</v>
       </c>
       <c r="AN33" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -4566,12 +4552,12 @@
         <v>0</v>
       </c>
       <c r="AN34" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
@@ -4688,12 +4674,12 @@
         <v>0</v>
       </c>
       <c r="AN35" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -4810,12 +4796,12 @@
         <v>0</v>
       </c>
       <c r="AN36" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -4932,12 +4918,12 @@
         <v>0</v>
       </c>
       <c r="AN37" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -5054,12 +5040,12 @@
         <v>0</v>
       </c>
       <c r="AN38" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -5176,12 +5162,12 @@
         <v>0</v>
       </c>
       <c r="AN39" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
@@ -5298,12 +5284,12 @@
         <v>0</v>
       </c>
       <c r="AN40" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
@@ -5420,12 +5406,12 @@
         <v>0</v>
       </c>
       <c r="AN41" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -5542,12 +5528,12 @@
         <v>0</v>
       </c>
       <c r="AN42" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -5664,12 +5650,12 @@
         <v>0</v>
       </c>
       <c r="AN43" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
@@ -5786,12 +5772,12 @@
         <v>0</v>
       </c>
       <c r="AN44" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -5908,12 +5894,12 @@
         <v>0</v>
       </c>
       <c r="AN45" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
@@ -6030,12 +6016,12 @@
         <v>0</v>
       </c>
       <c r="AN46" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -6152,12 +6138,12 @@
         <v>0</v>
       </c>
       <c r="AN47" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -6274,12 +6260,12 @@
         <v>0</v>
       </c>
       <c r="AN48" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -6396,12 +6382,12 @@
         <v>0</v>
       </c>
       <c r="AN49" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
@@ -6518,12 +6504,12 @@
         <v>0</v>
       </c>
       <c r="AN50" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -6640,12 +6626,12 @@
         <v>0</v>
       </c>
       <c r="AN51" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -6762,12 +6748,12 @@
         <v>0</v>
       </c>
       <c r="AN52" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -6884,12 +6870,12 @@
         <v>0</v>
       </c>
       <c r="AN53" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
@@ -7006,12 +6992,12 @@
         <v>0</v>
       </c>
       <c r="AN54" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
@@ -7128,12 +7114,12 @@
         <v>0</v>
       </c>
       <c r="AN55" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
@@ -7250,12 +7236,12 @@
         <v>0</v>
       </c>
       <c r="AN56" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B57" s="1">
         <v>0</v>
@@ -7372,12 +7358,12 @@
         <v>0</v>
       </c>
       <c r="AN57" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
@@ -7494,12 +7480,12 @@
         <v>0</v>
       </c>
       <c r="AN58" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
@@ -7616,12 +7602,12 @@
         <v>0</v>
       </c>
       <c r="AN59" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
@@ -7738,12 +7724,12 @@
         <v>0</v>
       </c>
       <c r="AN60" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
@@ -7860,12 +7846,12 @@
         <v>0</v>
       </c>
       <c r="AN61" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
@@ -7982,12 +7968,12 @@
         <v>0</v>
       </c>
       <c r="AN62" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
@@ -8104,12 +8090,12 @@
         <v>0</v>
       </c>
       <c r="AN63" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
@@ -8226,12 +8212,12 @@
         <v>0</v>
       </c>
       <c r="AN64" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
@@ -8348,12 +8334,12 @@
         <v>0</v>
       </c>
       <c r="AN65" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
@@ -8470,12 +8456,12 @@
         <v>0</v>
       </c>
       <c r="AN66" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B67" s="1">
         <v>0</v>
@@ -8592,12 +8578,12 @@
         <v>0</v>
       </c>
       <c r="AN67" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B68" s="1">
         <v>0</v>
@@ -8714,12 +8700,12 @@
         <v>0</v>
       </c>
       <c r="AN68" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B69" s="1">
         <v>0</v>
@@ -8836,12 +8822,12 @@
         <v>0</v>
       </c>
       <c r="AN69" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -8958,12 +8944,12 @@
         <v>0</v>
       </c>
       <c r="AN70" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B71" s="1">
         <v>0</v>
@@ -9080,12 +9066,12 @@
         <v>0</v>
       </c>
       <c r="AN71" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
@@ -9202,12 +9188,12 @@
         <v>0</v>
       </c>
       <c r="AN72" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B73" s="1">
         <v>0</v>
@@ -9324,12 +9310,12 @@
         <v>0</v>
       </c>
       <c r="AN73" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B74" s="1">
         <v>0</v>
@@ -9446,12 +9432,12 @@
         <v>0</v>
       </c>
       <c r="AN74" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B75" s="1">
         <v>0</v>
@@ -9568,12 +9554,12 @@
         <v>0</v>
       </c>
       <c r="AN75" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
@@ -9690,12 +9676,12 @@
         <v>0</v>
       </c>
       <c r="AN76" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B77" s="1">
         <v>0</v>
@@ -9812,12 +9798,12 @@
         <v>0</v>
       </c>
       <c r="AN77" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B78" s="1">
         <v>0</v>
@@ -9934,12 +9920,12 @@
         <v>0</v>
       </c>
       <c r="AN78" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B79" s="1">
         <v>0</v>
@@ -10056,12 +10042,12 @@
         <v>0</v>
       </c>
       <c r="AN79" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B80" s="1">
         <v>0</v>
@@ -10178,12 +10164,12 @@
         <v>0</v>
       </c>
       <c r="AN80" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B81" s="1">
         <v>0</v>
@@ -10300,12 +10286,12 @@
         <v>0</v>
       </c>
       <c r="AN81" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B82" s="1">
         <v>0</v>
@@ -10422,12 +10408,12 @@
         <v>0</v>
       </c>
       <c r="AN82" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B83" s="1">
         <v>0</v>
@@ -10544,12 +10530,12 @@
         <v>0</v>
       </c>
       <c r="AN83" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B84" s="1">
         <v>0</v>
@@ -10666,12 +10652,12 @@
         <v>0</v>
       </c>
       <c r="AN84" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B85" s="1">
         <v>0</v>
@@ -10788,12 +10774,12 @@
         <v>0</v>
       </c>
       <c r="AN85" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B86" s="1">
         <v>0</v>
@@ -10910,12 +10896,12 @@
         <v>0</v>
       </c>
       <c r="AN86" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B87" s="1">
         <v>0</v>
@@ -11032,12 +11018,12 @@
         <v>0</v>
       </c>
       <c r="AN87" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B88" s="1">
         <v>0</v>
@@ -11154,12 +11140,12 @@
         <v>0</v>
       </c>
       <c r="AN88" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B89" s="1">
         <v>0</v>
@@ -11276,12 +11262,12 @@
         <v>0</v>
       </c>
       <c r="AN89" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B90" s="1">
         <v>0</v>
@@ -11398,12 +11384,12 @@
         <v>0</v>
       </c>
       <c r="AN90" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B91" s="1">
         <v>0</v>
@@ -11520,12 +11506,12 @@
         <v>0</v>
       </c>
       <c r="AN91" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B92" s="1">
         <v>0</v>
@@ -11642,12 +11628,12 @@
         <v>0</v>
       </c>
       <c r="AN92" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B93" s="1">
         <v>0</v>
@@ -11764,12 +11750,12 @@
         <v>0</v>
       </c>
       <c r="AN93" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B94" s="1">
         <v>0</v>
@@ -11886,12 +11872,12 @@
         <v>0</v>
       </c>
       <c r="AN94" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B95" s="1">
         <v>0</v>
@@ -12008,12 +11994,12 @@
         <v>0</v>
       </c>
       <c r="AN95" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B96" s="1">
         <v>0</v>
@@ -12130,12 +12116,12 @@
         <v>0</v>
       </c>
       <c r="AN96" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B97" s="1">
         <v>0</v>
@@ -12252,12 +12238,12 @@
         <v>0</v>
       </c>
       <c r="AN97" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B98" s="1">
         <v>0</v>
@@ -12374,12 +12360,12 @@
         <v>0</v>
       </c>
       <c r="AN98" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B99" s="1">
         <v>0</v>
@@ -12496,12 +12482,12 @@
         <v>0</v>
       </c>
       <c r="AN99" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B100" s="1">
         <v>0</v>
@@ -12618,12 +12604,12 @@
         <v>0</v>
       </c>
       <c r="AN100" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B101" s="1">
         <v>0</v>
@@ -12740,12 +12726,12 @@
         <v>0</v>
       </c>
       <c r="AN101" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B102" s="1">
         <v>0</v>
@@ -12862,12 +12848,12 @@
         <v>0</v>
       </c>
       <c r="AN102" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B103" s="1">
         <v>0</v>
@@ -12984,12 +12970,12 @@
         <v>0</v>
       </c>
       <c r="AN103" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B104" s="1">
         <v>0</v>
@@ -13106,12 +13092,12 @@
         <v>0</v>
       </c>
       <c r="AN104" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B105" s="1">
         <v>0</v>
@@ -13228,12 +13214,12 @@
         <v>0</v>
       </c>
       <c r="AN105" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B106" s="1">
         <v>0</v>
@@ -13350,12 +13336,12 @@
         <v>0</v>
       </c>
       <c r="AN106" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B107" s="1">
         <v>0</v>
@@ -13472,12 +13458,12 @@
         <v>0</v>
       </c>
       <c r="AN107" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B108" s="1">
         <v>0</v>
@@ -13594,12 +13580,12 @@
         <v>0</v>
       </c>
       <c r="AN108" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B109" s="1">
         <v>0</v>
@@ -13716,12 +13702,12 @@
         <v>0</v>
       </c>
       <c r="AN109" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B110" s="1">
         <v>0</v>
@@ -13838,12 +13824,12 @@
         <v>0</v>
       </c>
       <c r="AN110" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B111" s="1">
         <v>0</v>
@@ -13960,12 +13946,12 @@
         <v>0</v>
       </c>
       <c r="AN111" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B112" s="1">
         <v>0</v>
@@ -14082,12 +14068,12 @@
         <v>0</v>
       </c>
       <c r="AN112" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B113" s="1">
         <v>0</v>
@@ -14204,12 +14190,12 @@
         <v>0</v>
       </c>
       <c r="AN113" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B114" s="1">
         <v>0</v>
@@ -14326,12 +14312,12 @@
         <v>0</v>
       </c>
       <c r="AN114" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B115" s="1">
         <v>0</v>
@@ -14448,12 +14434,12 @@
         <v>0</v>
       </c>
       <c r="AN115" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B116" s="1">
         <v>0</v>
@@ -14570,12 +14556,12 @@
         <v>0</v>
       </c>
       <c r="AN116" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B117" s="1">
         <v>0</v>
@@ -14692,12 +14678,12 @@
         <v>0</v>
       </c>
       <c r="AN117" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B118" s="1">
         <v>0</v>
@@ -14814,12 +14800,12 @@
         <v>0</v>
       </c>
       <c r="AN118" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B119" s="1">
         <v>0</v>
@@ -14936,12 +14922,12 @@
         <v>0</v>
       </c>
       <c r="AN119" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B120" s="1">
         <v>0</v>
@@ -15058,12 +15044,12 @@
         <v>0</v>
       </c>
       <c r="AN120" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B121" s="1">
         <v>0</v>
@@ -15180,12 +15166,12 @@
         <v>0</v>
       </c>
       <c r="AN121" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B122" s="1">
         <v>0</v>
@@ -15302,12 +15288,12 @@
         <v>0</v>
       </c>
       <c r="AN122" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B123" s="1">
         <v>0</v>
@@ -15424,12 +15410,12 @@
         <v>0</v>
       </c>
       <c r="AN123" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B124" s="1">
         <v>0</v>
@@ -15546,12 +15532,12 @@
         <v>0</v>
       </c>
       <c r="AN124" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B125" s="1">
         <v>0</v>
@@ -15668,12 +15654,12 @@
         <v>0</v>
       </c>
       <c r="AN125" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B126" s="1">
         <v>0</v>
@@ -15790,12 +15776,12 @@
         <v>0</v>
       </c>
       <c r="AN126" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B127" s="1">
         <v>0</v>
@@ -15912,12 +15898,12 @@
         <v>0</v>
       </c>
       <c r="AN127" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B128" s="1">
         <v>0</v>
@@ -16034,12 +16020,12 @@
         <v>0</v>
       </c>
       <c r="AN128" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B129" s="1">
         <v>0</v>
@@ -16156,12 +16142,12 @@
         <v>0</v>
       </c>
       <c r="AN129" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B130" s="1">
         <v>0</v>
@@ -16278,12 +16264,12 @@
         <v>0</v>
       </c>
       <c r="AN130" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B131" s="1">
         <v>0</v>
@@ -16400,12 +16386,12 @@
         <v>0</v>
       </c>
       <c r="AN131" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B132" s="1">
         <v>0</v>
@@ -16522,12 +16508,12 @@
         <v>0</v>
       </c>
       <c r="AN132" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B133" s="1">
         <v>0</v>
@@ -16644,12 +16630,12 @@
         <v>0</v>
       </c>
       <c r="AN133" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B134" s="1">
         <v>0</v>
@@ -16766,12 +16752,12 @@
         <v>0</v>
       </c>
       <c r="AN134" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B135" s="1">
         <v>0</v>
@@ -16888,12 +16874,12 @@
         <v>0</v>
       </c>
       <c r="AN135" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B136" s="1">
         <v>0</v>
@@ -17010,12 +16996,12 @@
         <v>0</v>
       </c>
       <c r="AN136" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B137" s="1">
         <v>0</v>
@@ -17132,12 +17118,12 @@
         <v>0</v>
       </c>
       <c r="AN137" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B138" s="1">
         <v>0</v>
@@ -17254,12 +17240,12 @@
         <v>0</v>
       </c>
       <c r="AN138" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B139" s="1">
         <v>0</v>
@@ -17376,12 +17362,12 @@
         <v>0</v>
       </c>
       <c r="AN139" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B140" s="1">
         <v>0</v>
@@ -17498,12 +17484,12 @@
         <v>0</v>
       </c>
       <c r="AN140" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B141" s="1">
         <v>0</v>
@@ -17620,12 +17606,12 @@
         <v>0</v>
       </c>
       <c r="AN141" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B142" s="1">
         <v>0</v>
@@ -17742,12 +17728,12 @@
         <v>0</v>
       </c>
       <c r="AN142" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B143" s="1">
         <v>0</v>
@@ -17864,12 +17850,12 @@
         <v>0</v>
       </c>
       <c r="AN143" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B144" s="1">
         <v>0</v>
@@ -17986,12 +17972,12 @@
         <v>0</v>
       </c>
       <c r="AN144" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B145" s="1">
         <v>0</v>
@@ -18108,12 +18094,12 @@
         <v>0</v>
       </c>
       <c r="AN145" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B146" s="1">
         <v>0</v>
@@ -18230,12 +18216,12 @@
         <v>0</v>
       </c>
       <c r="AN146" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B147" s="1">
         <v>0</v>
@@ -18352,12 +18338,12 @@
         <v>0</v>
       </c>
       <c r="AN147" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B148" s="1">
         <v>0</v>
@@ -18474,12 +18460,12 @@
         <v>0</v>
       </c>
       <c r="AN148" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B149" s="1">
         <v>0</v>
@@ -18596,12 +18582,12 @@
         <v>0</v>
       </c>
       <c r="AN149" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B150" s="1">
         <v>0</v>
@@ -18718,12 +18704,12 @@
         <v>0</v>
       </c>
       <c r="AN150" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B151" s="1">
         <v>0</v>
@@ -18840,12 +18826,12 @@
         <v>0</v>
       </c>
       <c r="AN151" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B152" s="1">
         <v>0</v>
@@ -18962,12 +18948,12 @@
         <v>0</v>
       </c>
       <c r="AN152" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B153" s="1">
         <v>0</v>
@@ -19084,12 +19070,12 @@
         <v>0</v>
       </c>
       <c r="AN153" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B154" s="1">
         <v>0</v>
@@ -19206,12 +19192,12 @@
         <v>0</v>
       </c>
       <c r="AN154" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B155" s="1">
         <v>0</v>
@@ -19328,12 +19314,12 @@
         <v>0</v>
       </c>
       <c r="AN155" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B156" s="1">
         <v>0</v>
@@ -19450,12 +19436,12 @@
         <v>0</v>
       </c>
       <c r="AN156" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B157" s="1">
         <v>0</v>
@@ -19572,12 +19558,12 @@
         <v>0</v>
       </c>
       <c r="AN157" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="158" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B158" s="1">
         <v>0</v>
@@ -19694,12 +19680,12 @@
         <v>0</v>
       </c>
       <c r="AN158" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="159" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B159" s="1">
         <v>0</v>
@@ -19816,12 +19802,12 @@
         <v>0</v>
       </c>
       <c r="AN159" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="160" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B160" s="1">
         <v>0</v>
@@ -19938,12 +19924,12 @@
         <v>0</v>
       </c>
       <c r="AN160" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B161" s="1">
         <v>0</v>
@@ -20060,12 +20046,12 @@
         <v>0</v>
       </c>
       <c r="AN161" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B162" s="1">
         <v>0</v>
@@ -20182,12 +20168,12 @@
         <v>0</v>
       </c>
       <c r="AN162" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B163" s="1">
         <v>0</v>
@@ -20304,12 +20290,12 @@
         <v>0</v>
       </c>
       <c r="AN163" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B164" s="1">
         <v>0</v>
@@ -20426,12 +20412,12 @@
         <v>0</v>
       </c>
       <c r="AN164" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B165" s="1">
         <v>0</v>
@@ -20548,12 +20534,12 @@
         <v>0</v>
       </c>
       <c r="AN165" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B166" s="1">
         <v>0</v>
@@ -20670,12 +20656,12 @@
         <v>0</v>
       </c>
       <c r="AN166" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B167" s="1">
         <v>0</v>
@@ -20792,12 +20778,12 @@
         <v>0</v>
       </c>
       <c r="AN167" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B168" s="1">
         <v>0</v>
@@ -20914,12 +20900,12 @@
         <v>0</v>
       </c>
       <c r="AN168" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B169" s="1">
         <v>0</v>
@@ -21036,12 +21022,12 @@
         <v>0</v>
       </c>
       <c r="AN169" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B170" s="1">
         <v>0</v>
@@ -21158,12 +21144,12 @@
         <v>0</v>
       </c>
       <c r="AN170" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B171" s="1">
         <v>0</v>
@@ -21280,12 +21266,12 @@
         <v>0</v>
       </c>
       <c r="AN171" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B172" s="1">
         <v>0</v>
@@ -21402,12 +21388,12 @@
         <v>0</v>
       </c>
       <c r="AN172" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B173" s="1">
         <v>0</v>
@@ -21524,12 +21510,12 @@
         <v>0</v>
       </c>
       <c r="AN173" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="174" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B174" s="1">
         <v>0</v>
@@ -21646,12 +21632,12 @@
         <v>0</v>
       </c>
       <c r="AN174" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B175" s="1">
         <v>0</v>
@@ -21768,12 +21754,12 @@
         <v>0</v>
       </c>
       <c r="AN175" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B176" s="1">
         <v>0</v>
@@ -21890,12 +21876,12 @@
         <v>0</v>
       </c>
       <c r="AN176" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B177" s="1">
         <v>0</v>
@@ -22012,12 +21998,12 @@
         <v>0</v>
       </c>
       <c r="AN177" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B178" s="1">
         <v>0</v>
@@ -22134,12 +22120,12 @@
         <v>0</v>
       </c>
       <c r="AN178" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="179" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B179" s="1">
         <v>0</v>
@@ -22256,12 +22242,12 @@
         <v>0</v>
       </c>
       <c r="AN179" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B180" s="1">
         <v>0</v>
@@ -22378,12 +22364,12 @@
         <v>0</v>
       </c>
       <c r="AN180" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="181" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B181" s="1">
         <v>0</v>
@@ -22500,12 +22486,12 @@
         <v>0</v>
       </c>
       <c r="AN181" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B182" s="1">
         <v>0</v>
@@ -22622,12 +22608,12 @@
         <v>0</v>
       </c>
       <c r="AN182" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="183" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B183" s="1">
         <v>0</v>
@@ -22744,12 +22730,12 @@
         <v>0</v>
       </c>
       <c r="AN183" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B184" s="1">
         <v>0</v>
@@ -22866,12 +22852,12 @@
         <v>0</v>
       </c>
       <c r="AN184" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B185" s="1">
         <v>0</v>
@@ -22988,12 +22974,12 @@
         <v>0</v>
       </c>
       <c r="AN185" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="186" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B186" s="1">
         <v>0</v>
@@ -23110,12 +23096,12 @@
         <v>0</v>
       </c>
       <c r="AN186" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B187" s="1">
         <v>0</v>
@@ -23232,12 +23218,12 @@
         <v>0</v>
       </c>
       <c r="AN187" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B188" s="1">
         <v>0</v>
@@ -23354,12 +23340,12 @@
         <v>0</v>
       </c>
       <c r="AN188" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="189" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B189" s="1">
         <v>0</v>
@@ -23476,12 +23462,12 @@
         <v>0</v>
       </c>
       <c r="AN189" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B190" s="1">
         <v>0</v>
@@ -23598,12 +23584,12 @@
         <v>0</v>
       </c>
       <c r="AN190" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B191" s="1">
         <v>0</v>
@@ -23720,12 +23706,12 @@
         <v>0</v>
       </c>
       <c r="AN191" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="192" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B192" s="1">
         <v>0</v>
@@ -23842,12 +23828,12 @@
         <v>0</v>
       </c>
       <c r="AN192" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B193" s="1">
         <v>0</v>
@@ -23964,12 +23950,12 @@
         <v>0</v>
       </c>
       <c r="AN193" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B194" s="1">
         <v>0</v>
@@ -24086,12 +24072,12 @@
         <v>0</v>
       </c>
       <c r="AN194" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="195" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B195" s="1">
         <v>0</v>
@@ -24208,12 +24194,12 @@
         <v>0</v>
       </c>
       <c r="AN195" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="196" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B196" s="1">
         <v>0</v>
@@ -24330,12 +24316,12 @@
         <v>0</v>
       </c>
       <c r="AN196" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B197" s="1">
         <v>0</v>
@@ -24452,12 +24438,12 @@
         <v>0</v>
       </c>
       <c r="AN197" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="198" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B198" s="1">
         <v>0</v>
@@ -24574,12 +24560,12 @@
         <v>0</v>
       </c>
       <c r="AN198" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="199" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B199" s="1">
         <v>0</v>
@@ -24696,12 +24682,12 @@
         <v>0</v>
       </c>
       <c r="AN199" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="200" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B200" s="1">
         <v>0</v>
@@ -24818,12 +24804,12 @@
         <v>0</v>
       </c>
       <c r="AN200" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B201" s="1">
         <v>0</v>
@@ -24940,12 +24926,12 @@
         <v>0</v>
       </c>
       <c r="AN201" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="202" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B202" s="1">
         <v>0</v>
@@ -25062,12 +25048,12 @@
         <v>0</v>
       </c>
       <c r="AN202" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="203" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B203" s="1">
         <v>0</v>
@@ -25184,12 +25170,12 @@
         <v>0</v>
       </c>
       <c r="AN203" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="204" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B204" s="1">
         <v>0</v>
@@ -25306,12 +25292,12 @@
         <v>0</v>
       </c>
       <c r="AN204" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="205" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B205" s="1">
         <v>0</v>
@@ -25428,12 +25414,12 @@
         <v>0</v>
       </c>
       <c r="AN205" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="206" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B206" s="1">
         <v>0</v>
@@ -25550,12 +25536,12 @@
         <v>0</v>
       </c>
       <c r="AN206" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="207" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B207" s="1">
         <v>0</v>
@@ -25672,12 +25658,12 @@
         <v>0</v>
       </c>
       <c r="AN207" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="208" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B208" s="1">
         <v>0</v>
@@ -25794,12 +25780,12 @@
         <v>0</v>
       </c>
       <c r="AN208" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="209" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B209" s="1">
         <v>0</v>
@@ -25916,12 +25902,12 @@
         <v>0</v>
       </c>
       <c r="AN209" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="210" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B210" s="1">
         <v>0</v>
@@ -26038,12 +26024,12 @@
         <v>0</v>
       </c>
       <c r="AN210" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="211" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B211" s="1">
         <v>0</v>
@@ -26160,12 +26146,12 @@
         <v>0</v>
       </c>
       <c r="AN211" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="212" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B212" s="1">
         <v>0</v>
@@ -26282,12 +26268,12 @@
         <v>0</v>
       </c>
       <c r="AN212" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="213" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B213" s="1">
         <v>0</v>
@@ -26404,12 +26390,12 @@
         <v>0</v>
       </c>
       <c r="AN213" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="214" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B214" s="1">
         <v>0</v>
@@ -26526,12 +26512,12 @@
         <v>0</v>
       </c>
       <c r="AN214" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="215" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B215" s="1">
         <v>0</v>
@@ -26648,12 +26634,12 @@
         <v>0</v>
       </c>
       <c r="AN215" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="216" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B216" s="1">
         <v>0</v>
@@ -26770,12 +26756,12 @@
         <v>0</v>
       </c>
       <c r="AN216" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="217" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B217" s="1">
         <v>0</v>
@@ -26892,12 +26878,12 @@
         <v>0</v>
       </c>
       <c r="AN217" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="218" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B218" s="1">
         <v>0</v>
@@ -27014,12 +27000,12 @@
         <v>0</v>
       </c>
       <c r="AN218" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="219" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B219" s="1">
         <v>0</v>
@@ -27136,12 +27122,12 @@
         <v>0</v>
       </c>
       <c r="AN219" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="220" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B220" s="1">
         <v>0</v>
@@ -27258,12 +27244,12 @@
         <v>0</v>
       </c>
       <c r="AN220" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="221" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B221" s="1">
         <v>0</v>
@@ -27380,12 +27366,12 @@
         <v>0</v>
       </c>
       <c r="AN221" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="222" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B222" s="1">
         <v>0</v>
@@ -27502,12 +27488,12 @@
         <v>0</v>
       </c>
       <c r="AN222" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="223" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B223" s="1">
         <v>0</v>
@@ -27624,12 +27610,12 @@
         <v>0</v>
       </c>
       <c r="AN223" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="224" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B224" s="1">
         <v>0</v>
@@ -27746,12 +27732,12 @@
         <v>0</v>
       </c>
       <c r="AN224" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="225" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B225" s="1">
         <v>0</v>
@@ -27868,12 +27854,12 @@
         <v>0</v>
       </c>
       <c r="AN225" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="226" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B226" s="1">
         <v>0</v>
@@ -27990,12 +27976,12 @@
         <v>0</v>
       </c>
       <c r="AN226" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="227" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B227" s="1">
         <v>0</v>
@@ -28112,12 +28098,12 @@
         <v>0</v>
       </c>
       <c r="AN227" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="228" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B228" s="1">
         <v>0</v>
@@ -28234,12 +28220,12 @@
         <v>0</v>
       </c>
       <c r="AN228" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="229" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B229" s="1">
         <v>0</v>
@@ -28356,12 +28342,12 @@
         <v>0</v>
       </c>
       <c r="AN229" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="230" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B230" s="1">
         <v>0</v>
@@ -28478,12 +28464,12 @@
         <v>0</v>
       </c>
       <c r="AN230" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="231" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B231" s="1">
         <v>0</v>
@@ -28600,12 +28586,12 @@
         <v>0</v>
       </c>
       <c r="AN231" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="232" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B232" s="1">
         <v>0</v>
@@ -28722,12 +28708,12 @@
         <v>0</v>
       </c>
       <c r="AN232" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="233" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B233" s="1">
         <v>0</v>
@@ -28844,12 +28830,12 @@
         <v>0</v>
       </c>
       <c r="AN233" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="234" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B234" s="1">
         <v>0</v>
@@ -28966,12 +28952,12 @@
         <v>0</v>
       </c>
       <c r="AN234" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="235" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B235" s="1">
         <v>0</v>
@@ -29088,12 +29074,12 @@
         <v>0</v>
       </c>
       <c r="AN235" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="236" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B236" s="1">
         <v>0</v>
@@ -29210,12 +29196,12 @@
         <v>0</v>
       </c>
       <c r="AN236" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="237" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B237" s="1">
         <v>0</v>
@@ -29332,12 +29318,12 @@
         <v>0</v>
       </c>
       <c r="AN237" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="238" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B238" s="1">
         <v>0</v>
@@ -29454,12 +29440,12 @@
         <v>0</v>
       </c>
       <c r="AN238" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="239" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B239" s="1">
         <v>0</v>
@@ -29576,12 +29562,12 @@
         <v>0</v>
       </c>
       <c r="AN239" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="240" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B240" s="1">
         <v>0</v>
@@ -29698,12 +29684,12 @@
         <v>0</v>
       </c>
       <c r="AN240" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="241" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B241" s="1">
         <v>0</v>
@@ -29820,12 +29806,12 @@
         <v>0</v>
       </c>
       <c r="AN241" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="242" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B242" s="1">
         <v>0</v>
@@ -29942,12 +29928,12 @@
         <v>0</v>
       </c>
       <c r="AN242" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="243" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B243" s="1">
         <v>0</v>
@@ -30064,12 +30050,12 @@
         <v>0</v>
       </c>
       <c r="AN243" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="244" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B244" s="1">
         <v>0</v>
@@ -30186,12 +30172,12 @@
         <v>0</v>
       </c>
       <c r="AN244" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="245" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B245" s="1">
         <v>0</v>
@@ -30308,12 +30294,12 @@
         <v>0</v>
       </c>
       <c r="AN245" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="246" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B246" s="1">
         <v>0</v>
@@ -30430,12 +30416,12 @@
         <v>0</v>
       </c>
       <c r="AN246" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="247" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B247" s="1">
         <v>0</v>
@@ -30552,12 +30538,12 @@
         <v>0</v>
       </c>
       <c r="AN247" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="248" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B248" s="1">
         <v>0</v>
@@ -30674,12 +30660,12 @@
         <v>0</v>
       </c>
       <c r="AN248" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B249" s="1">
         <v>0</v>
@@ -30796,12 +30782,12 @@
         <v>0</v>
       </c>
       <c r="AN249" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="250" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B250" s="1">
         <v>0</v>
@@ -30918,12 +30904,12 @@
         <v>0</v>
       </c>
       <c r="AN250" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="251" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B251" s="1">
         <v>0</v>
@@ -31040,12 +31026,12 @@
         <v>0</v>
       </c>
       <c r="AN251" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="252" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B252" s="1">
         <v>0</v>
@@ -31162,12 +31148,12 @@
         <v>0</v>
       </c>
       <c r="AN252" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="253" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B253" s="1">
         <v>0</v>
@@ -31284,12 +31270,12 @@
         <v>0</v>
       </c>
       <c r="AN253" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="254" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B254" s="1">
         <v>0</v>
@@ -31406,12 +31392,12 @@
         <v>0</v>
       </c>
       <c r="AN254" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="255" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B255" s="1">
         <v>0</v>
@@ -31528,12 +31514,12 @@
         <v>0</v>
       </c>
       <c r="AN255" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="256" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B256" s="1">
         <v>0</v>
@@ -31650,12 +31636,12 @@
         <v>0</v>
       </c>
       <c r="AN256" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="257" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B257" s="1">
         <v>0</v>
@@ -31772,12 +31758,12 @@
         <v>0</v>
       </c>
       <c r="AN257" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="258" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B258" s="1">
         <v>0</v>
@@ -31894,12 +31880,12 @@
         <v>0</v>
       </c>
       <c r="AN258" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="259" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B259" s="1">
         <v>0</v>
@@ -32016,12 +32002,12 @@
         <v>0</v>
       </c>
       <c r="AN259" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B260" s="1">
         <v>0</v>
@@ -32138,12 +32124,12 @@
         <v>0</v>
       </c>
       <c r="AN260" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="261" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B261" s="1">
         <v>0</v>
@@ -32260,12 +32246,12 @@
         <v>0</v>
       </c>
       <c r="AN261" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="262" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B262" s="1">
         <v>0</v>
@@ -32382,12 +32368,12 @@
         <v>0</v>
       </c>
       <c r="AN262" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="263" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B263" s="1">
         <v>0</v>
@@ -32504,12 +32490,12 @@
         <v>0</v>
       </c>
       <c r="AN263" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="264" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B264" s="1">
         <v>0</v>
@@ -32626,12 +32612,12 @@
         <v>0</v>
       </c>
       <c r="AN264" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="265" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B265" s="1">
         <v>0</v>
@@ -32748,12 +32734,12 @@
         <v>0</v>
       </c>
       <c r="AN265" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="266" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B266" s="1">
         <v>0</v>
@@ -32870,12 +32856,12 @@
         <v>0</v>
       </c>
       <c r="AN266" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="267" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B267" s="1">
         <v>0</v>
@@ -32992,12 +32978,12 @@
         <v>0</v>
       </c>
       <c r="AN267" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="268" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B268" s="1">
         <v>0</v>
@@ -33114,12 +33100,12 @@
         <v>0</v>
       </c>
       <c r="AN268" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="269" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B269" s="1">
         <v>0</v>
@@ -33236,12 +33222,12 @@
         <v>0</v>
       </c>
       <c r="AN269" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="270" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B270" s="1">
         <v>0</v>
@@ -33358,12 +33344,12 @@
         <v>0</v>
       </c>
       <c r="AN270" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="271" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B271" s="1">
         <v>0</v>
@@ -33480,12 +33466,12 @@
         <v>0</v>
       </c>
       <c r="AN271" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="272" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B272" s="1">
         <v>0</v>
@@ -33602,12 +33588,12 @@
         <v>0</v>
       </c>
       <c r="AN272" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="273" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B273" s="1">
         <v>0</v>
@@ -33724,12 +33710,12 @@
         <v>0</v>
       </c>
       <c r="AN273" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="274" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B274" s="1">
         <v>0</v>
@@ -33846,12 +33832,12 @@
         <v>0</v>
       </c>
       <c r="AN274" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="275" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B275" s="1">
         <v>0</v>
@@ -33968,12 +33954,12 @@
         <v>0</v>
       </c>
       <c r="AN275" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="276" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B276" s="1">
         <v>0</v>
@@ -34090,12 +34076,12 @@
         <v>0</v>
       </c>
       <c r="AN276" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="277" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B277" s="1">
         <v>0</v>
@@ -34212,12 +34198,12 @@
         <v>0</v>
       </c>
       <c r="AN277" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="278" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B278" s="1">
         <v>2</v>
@@ -34334,12 +34320,12 @@
         <v>2</v>
       </c>
       <c r="AN278" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="279" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B279" s="1">
         <v>0</v>
@@ -34456,12 +34442,12 @@
         <v>0</v>
       </c>
       <c r="AN279" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="280" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B280" s="1">
         <v>0</v>
@@ -34578,12 +34564,12 @@
         <v>0</v>
       </c>
       <c r="AN280" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="281" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B281" s="1">
         <v>0</v>
@@ -34700,12 +34686,12 @@
         <v>0</v>
       </c>
       <c r="AN281" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="282" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B282" s="1">
         <v>0</v>
@@ -34822,12 +34808,12 @@
         <v>0</v>
       </c>
       <c r="AN282" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="283" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B283" s="1">
         <v>0</v>
@@ -34944,12 +34930,12 @@
         <v>0</v>
       </c>
       <c r="AN283" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="284" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B284" s="1">
         <v>0</v>
@@ -35066,12 +35052,12 @@
         <v>0</v>
       </c>
       <c r="AN284" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="285" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B285" s="1">
         <v>0</v>
@@ -35188,12 +35174,12 @@
         <v>0</v>
       </c>
       <c r="AN285" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="286" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B286" s="1">
         <v>0</v>
@@ -35310,12 +35296,12 @@
         <v>0</v>
       </c>
       <c r="AN286" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="287" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B287" s="1">
         <v>0</v>
@@ -35432,12 +35418,12 @@
         <v>0</v>
       </c>
       <c r="AN287" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="288" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B288" s="1">
         <v>0</v>
@@ -35554,12 +35540,12 @@
         <v>0</v>
       </c>
       <c r="AN288" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="289" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B289" s="1">
         <v>0</v>
@@ -35676,129 +35662,129 @@
         <v>0</v>
       </c>
       <c r="AN289" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="290" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AE290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN290" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="291" spans="1:40" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -37023,11 +37009,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:AN300">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>2</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix map data, fix lazer error
</commit_message>
<xml_diff>
--- a/Project2/map/map_stage0.xlsx
+++ b/Project2/map/map_stage0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JumpKing\Project2\map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C366973B-AFDA-4A69-A934-FCE8CDC82136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAFFC73-B46E-4C94-AD6F-4C5783E39A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{43B2A935-9574-4456-95D9-363CC87949CB}"/>
+    <workbookView xWindow="3375" yWindow="4545" windowWidth="18000" windowHeight="9810" xr2:uid="{43B2A935-9574-4456-95D9-363CC87949CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFF67B08-2CB8-4D9E-8CCD-07B2A0732180}">
   <dimension ref="A1:AN300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="69" workbookViewId="0">
-      <selection activeCell="AR280" sqref="AR280"/>
+    <sheetView tabSelected="1" zoomScale="48" workbookViewId="0">
+      <selection activeCell="AN300" sqref="A1:AN300"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="24.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -34206,7 +34206,7 @@
         <v>6</v>
       </c>
       <c r="B278" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C278" s="1">
         <v>2</v>
@@ -34230,7 +34230,7 @@
         <v>2</v>
       </c>
       <c r="J278" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K278" s="1">
         <v>0</v>
@@ -34293,7 +34293,7 @@
         <v>0</v>
       </c>
       <c r="AE278" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AF278" s="1">
         <v>2</v>
@@ -34317,7 +34317,7 @@
         <v>2</v>
       </c>
       <c r="AM278" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AN278" s="1">
         <v>10</v>
@@ -34980,7 +34980,7 @@
         <v>0</v>
       </c>
       <c r="P284" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Q284" s="1">
         <v>2</v>
@@ -35004,7 +35004,7 @@
         <v>2</v>
       </c>
       <c r="X284" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y284" s="1">
         <v>0</v>

</xml_diff>